<commit_message>
Add hooks, rename product data repository, add product_attribute_repository
</commit_message>
<xml_diff>
--- a/addons/product_mesquita/data/product_data.xlsx
+++ b/addons/product_mesquita/data/product_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="product.attribute" sheetId="1" state="visible" r:id="rId3"/>
@@ -22,276 +22,535 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="185">
+  <si>
+    <t xml:space="preserve">ext_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">create_variant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">display_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_ancho_pl_mt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANCHO_PL_MT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dynamic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_alto_pl_mt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTO_PL_MT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_tipo_de_marco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TIPO_DE_MARCO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">radio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_sentido_de_apertura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SENTIDO_DE_APERTURA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ext_attribute_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">is_custom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_ancho_pl_500_mt_600</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANCHO PL: 500MM, ANCHO MT: 600MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_ancho_pl_550_mt_650</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANCHO PL: 550MM, ANCHO MT: 650MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_ancho_pl_600_mt_700</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANCHO PL: 600MM, ANCHO MT: 700MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_ancho_pl_650_mt_750</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANCHO PL: 650MM, ANCHO MT: 750MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_ancho_pl_700_mt_800</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANCHO PL: 700MM, ANCHO MT: 800MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_ancho_pl_750_mt_850</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANCHO PL: 750MM, ANCHO MT: 850MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_ancho_pl_800_mt_900</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANCHO PL: 800MM, ANCHO MT: 900MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_ancho_pl_850_mt_950</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANCHO PL: 850MM, ANCHO MT: 950MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_ancho_pl_900_mt_1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANCHO PL: 900MM, ANCHO MT: 1000MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_ancho_pl_950_mt_1050</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANCHO PL: 950MM, ANCHO MT: 1050MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_ancho_pl_1000_mt_1100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANCHO PL: 1000MM, ANCHO MT: 1100MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_ancho_pl_1050_mt_1150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANCHO PL: 1050MM, ANCHO MT: 1150MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_ancho_pl_1100_mt_1200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANCHO PL: 1100MM, ANCHO MT: 1200MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_ancho_pl_1150_mt_1250</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANCHO PL: 1150MM, ANCHO MT: 1250MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_ancho_pl_1200_mt_1300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANCHO PL: 1200MM, ANCHO MT: 1300MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_ancho_pl_1250_mt_1350</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANCHO PL: 1250MM, ANCHO MT: 1350MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_ancho_pl_1300_mt_1400</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANCHO PL: 1300MM, ANCHO MT: 1400MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_ancho_pl_1350_mt_1450</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANCHO PL: 1350MM, ANCHO MT: 1450MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_ancho_pl_1400_mt_1500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANCHO PL: 1400MM, ANCHO MT: 1500MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_ancho_pl_1450_mt_1550</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANCHO PL: 1450MM, ANCHO MT: 1550MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_ancho_pl_1500_mt_1600</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANCHO PL: 1500MM, ANCHO MT: 1600MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_ancho_pl_1550_mt_1650</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANCHO PL: 1550MM, ANCHO MT: 1650MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_ancho_pl_1600_mt_1700</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANCHO PL: 1600MM, ANCHO MT: 1700MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_ancho_pl_1650_mt_1750</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANCHO PL: 1650MM, ANCHO MT: 1750MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_ancho_pl_1700_mt_1800</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANCHO PL: 1700MM, ANCHO MT: 1800MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_ancho_pl_1750_mt_1850</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANCHO PL: 1750MM, ANCHO MT: 1850MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_ancho_pl_1800_mt_1900</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANCHO PL: 1800MM, ANCHO MT: 1900MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_ancho_pl_1850_mt_1950</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANCHO PL: 1850MM, ANCHO MT: 1950MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_ancho_pl_1900_mt_2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANCHO PL: 1900MM, ANCHO MT: 2000MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_ancho_pl_1950_mt_2050</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANCHO PL: 1950MM, ANCHO MT: 2050MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_ancho_pl_2000_mt_2100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANCHO PL: 2000MM, ANCHO MT: 2100MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_ancho_pl_2050_mt_2150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANCHO PL: 2050MM, ANCHO MT: 2150MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_ancho_pl_2100_mt_2200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANCHO PL: 2100MM, ANCHO MT: 2200MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_ancho_pl_2150_mt_2250</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANCHO PL: 2150MM, ANCHO MT: 2250MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_ancho_pl_2200_mt_2300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANCHO PL: 2200MM, ANCHO MT: 2300MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_alto_pl_500_mt_550</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTO PL: 500MM, ALTO MT: 550MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_alto_pl_550_mt_600</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTO PL: 550MM, ALTO MT: 600MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_alto_pl_600_mt_650</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTO PL: 600MM, ALTO MT: 650MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_alto_pl_650_mt_700</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTO PL: 650MM, ALTO MT: 700MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_alto_pl_700_mt_750</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTO PL: 700MM, ALTO MT: 750MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_alto_pl_750_mt_800</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTO PL: 750MM, ALTO MT: 800MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_alto_pl_800_mt_850</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTO PL: 800MM, ALTO MT: 850MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_alto_pl_850_mt_900</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTO PL: 850MM, ALTO MT: 900MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_alto_pl_900_mt_950</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTO PL: 900MM, ALTO MT: 950MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_alto_pl_950_mt_1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTO PL: 950MM, ALTO MT: 1000MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_alto_pl_1000_mt_1050</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTO PL: 1000MM, ALTO MT: 1050MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_alto_pl_1050_mt_1100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTO PL: 1050MM, ALTO MT: 1100MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_alto_pl_1100_mt_1150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTO PL: 1100MM, ALTO MT: 1150MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_alto_pl_1150_mt_1200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTO PL: 1150MM, ALTO MT: 1200MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_alto_pl_1200_mt_1250</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTO PL: 1200MM, ALTO MT: 1250MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_alto_pl_1250_mt_1300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTO PL: 1250MM, ALTO MT: 1300MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_alto_pl_1300_mt_1350</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTO PL: 1300MM, ALTO MT: 1350MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_alto_pl_1350_mt_1400</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTO PL: 1350MM, ALTO MT: 1400MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_alto_pl_1400_mt_1450</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTO PL: 1400MM, ALTO MT: 1450MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_alto_pl_1450_mt_1500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTO PL: 1450MM, ALTO MT: 1500MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_alto_pl_1500_mt_1550</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTO PL: 1500MM, ALTO MT: 1550MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_alto_pl_1550_mt_1600</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTO PL: 1550MM, ALTO MT: 1600MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_alto_pl_1600_mt_1650</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTO PL: 1600MM, ALTO MT: 1650MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_alto_pl_1650_mt_1700</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTO PL: 1650MM, ALTO MT: 1700MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_alto_pl_1700_mt_1750</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTO PL: 1700MM, ALTO MT: 1750MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_alto_pl_1750_mt_1800</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTO PL: 1750MM, ALTO MT: 1800MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_alto_pl_1800_mt_1850</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTO PL: 1800MM, ALTO MT: 1850MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_alto_pl_1850_mt_1900</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTO PL: 1850MM, ALTO MT: 1900MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_alto_pl_1900_mt_1950</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTO PL: 1900MM, ALTO MT: 1950MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_alto_pl_1950_mt_2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTO PL: 1950MM, ALTO MT: 2000MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_alto_pl_2000_mt_2050</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTO PL: 2000MM, ALTO MT: 2050MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_alto_pl_2050_mt_2100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTO PL: 2050MM, ALTO MT: 2100MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_alto_pl_2100_mt_2150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTO PL: 2100MM, ALTO MT: 2150MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_alto_pl_2150_mt_2200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTO PL: 2150MM, ALTO MT: 2200MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_alto_pl_2200_mt_2250</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTO PL: 2200MM, ALTO MT: 2250MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_alto_pl_2250_mt_2300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTO PL: 2250MM, ALTO MT: 2300MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_alto_pl_2300_mt_2350</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTO PL: 2300MM, ALTO MT: 2350MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_alto_pl_2350_mt_2400</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTO PL: 2350MM, ALTO MT: 2400MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_attribute_value_alto_pl_2400_mt_2450</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTO PL: 2400MM, ALTO MT: 2450MM</t>
+  </si>
   <si>
     <t xml:space="preserve">id</t>
   </si>
   <si>
-    <t xml:space="preserve">name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">create_variant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">display_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_attribute_ancho_pl_mt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANCHO_PL_MT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">always</t>
-  </si>
-  <si>
-    <t xml:space="preserve">select</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_attribute_alto_pl_mt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALTO_PL_MT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_attribute_tipo_de_marco</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TIPO_DE_MARCO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">radio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_attribute_sentido_de_apertura</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SENTIDO_DE_APERTURA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">attribute_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">is_custom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_attribute_value_ancho_pl_mt_500_600</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANCHO PL: 500MM, ANCHO MT: 600MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_attribute_value_ancho_pl_mt_550_650</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANCHO PL: 550MM, ANCHO MT: 650MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_attribute_value_ancho_pl_mt_600_700</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANCHO PL: 600MM, ANCHO MT: 700MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_attribute_value_ancho_pl_mt_650_750</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANCHO PL: 650MM, ANCHO MT: 750MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_attribute_value_ancho_pl_mt_700_800</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANCHO PL: 700MM, ANCHO MT: 800MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_attribute_value_ancho_pl_mt_750_850</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANCHO PL: 750MM, ANCHO MT: 850MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_attribute_value_ancho_pl_mt_800_900</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANCHO PL: 800MM, ANCHO MT: 900MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_attribute_value_ancho_pl_mt_850_950</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANCHO PL: 850MM, ANCHO MT: 950MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_attribute_value_ancho_pl_mt_900_1000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANCHO PL: 900MM, ANCHO MT: 1000MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_attribute_value_ancho_pl_mt_950_1050</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANCHO PL: 950MM, ANCHO MT: 1050MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_attribute_value_ancho_pl_mt_1000_1100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANCHO PL: 1000MM, ANCHO MT: 1100MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_attribute_value_ancho_pl_mt_1050_1150</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANCHO PL: 1050MM, ANCHO MT: 1150MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_attribute_value_ancho_pl_mt_1100_1200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANCHO PL: 1100MM, ANCHO MT: 1200MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_attribute_value_ancho_pl_mt_1150_1250</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANCHO PL: 1150MM, ANCHO MT: 1250MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_attribute_value_ancho_pl_mt_1200_1300</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANCHO PL: 1200MM, ANCHO MT: 1300MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_attribute_value_ancho_pl_mt_1250_1350</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANCHO PL: 1250MM, ANCHO MT: 1350MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_attribute_value_ancho_pl_mt_1300_1400</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANCHO PL: 1300MM, ANCHO MT: 1400MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_attribute_value_ancho_pl_mt_1350_1450</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANCHO PL: 1350MM, ANCHO MT: 1450MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_attribute_value_ancho_pl_mt_1400_1500</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANCHO PL: 1400MM, ANCHO MT: 1500MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_attribute_value_ancho_pl_mt_1450_1550</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANCHO PL: 1450MM, ANCHO MT: 1550MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_attribute_value_ancho_pl_mt_1500_1600</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANCHO PL: 1500MM, ANCHO MT: 1600MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_attribute_value_ancho_pl_mt_1550_1650</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANCHO PL: 1550MM, ANCHO MT: 1650MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_attribute_value_ancho_pl_mt_1600_1700</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANCHO PL: 1600MM, ANCHO MT: 1700MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_attribute_value_ancho_pl_mt_1650_1750</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANCHO PL: 1650MM, ANCHO MT: 1750MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_attribute_value_ancho_pl_mt_1700_1800</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANCHO PL: 1700MM, ANCHO MT: 1800MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_attribute_value_ancho_pl_mt_1750_1850</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANCHO PL: 1750MM, ANCHO MT: 1850MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_attribute_value_ancho_pl_mt_1800_1900</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANCHO PL: 1800MM, ANCHO MT: 1900MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_attribute_value_ancho_pl_mt_1850_1950</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANCHO PL: 1850MM, ANCHO MT: 1950MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_attribute_value_ancho_pl_mt_1900_2000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANCHO PL: 1900MM, ANCHO MT: 2000MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_attribute_value_ancho_pl_mt_1950_2050</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANCHO PL: 1950MM, ANCHO MT: 2050MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_attribute_value_ancho_pl_mt_2000_2100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANCHO PL: 2000MM, ANCHO MT: 2100MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_attribute_value_ancho_pl_mt_2050_2150</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANCHO PL: 2050MM, ANCHO MT: 2150MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_attribute_value_ancho_pl_mt_2100_2200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANCHO PL: 2100MM, ANCHO MT: 2200MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_attribute_value_ancho_pl_mt_2150_2250</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANCHO PL: 2150MM, ANCHO MT: 2250MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_attribute_value_ancho_pl_mt_2200_2300</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANCHO PL: 2200MM, ANCHO MT: 2300MM</t>
-  </si>
-  <si>
     <t xml:space="preserve">description</t>
   </si>
   <si>
+    <t xml:space="preserve">ext_attribute_ids</t>
+  </si>
+  <si>
     <t xml:space="preserve">product_template_rf_30_lite</t>
   </si>
   <si>
     <t xml:space="preserve">PUERTA RF30 LITE</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">product_attribute_ancho_pl_mt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">product_attribute_alto_pl_mt</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">product_template_rf_30_plus</t>
@@ -368,8 +627,8 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -424,22 +683,22 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -568,19 +827,19 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="40.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -589,7 +848,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -600,24 +859,24 @@
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
     </row>
@@ -628,10 +887,10 @@
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -642,10 +901,10 @@
       <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -665,10 +924,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D75"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B43" activeCellId="0" sqref="B43"/>
+      <selection pane="topLeft" activeCell="C37" activeCellId="0" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -679,10 +938,10 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1213,6 +1472,591 @@
         <v>4</v>
       </c>
       <c r="D36" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D45" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D46" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D51" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D52" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D53" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D54" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D55" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D56" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D57" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D58" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D59" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D60" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D61" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D62" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D63" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D64" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D65" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D66" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D67" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D68" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D69" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D70" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D71" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D72" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D73" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D74" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D75" s="5" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1233,10 +2077,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1244,105 +2088,133 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="33.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
+      <c r="A1" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>87</v>
+      <c r="C1" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>89</v>
+        <v>168</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>91</v>
+        <v>171</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>93</v>
+        <v>173</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>95</v>
+        <v>175</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>97</v>
+        <v>177</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>99</v>
+        <v>179</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>101</v>
+        <v>181</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>103</v>
+        <v>183</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add ProductTemplate repository, load product.template and .attribute.line via ORM
</commit_message>
<xml_diff>
--- a/addons/product_mesquita/data/product_data.xlsx
+++ b/addons/product_mesquita/data/product_data.xlsx
@@ -11,6 +11,7 @@
     <sheet name="product.attribute" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="product.attribute.value" sheetId="2" state="visible" r:id="rId4"/>
     <sheet name="product.template" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="product.template.attribute.line" sheetId="4" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,9 +23,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="185">
-  <si>
-    <t xml:space="preserve">ext_id</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="168">
+  <si>
+    <t xml:space="preserve">id</t>
   </si>
   <si>
     <t xml:space="preserve">name</t>
@@ -54,22 +55,7 @@
     <t xml:space="preserve">ALTO_PL_MT</t>
   </si>
   <si>
-    <t xml:space="preserve">product_attribute_tipo_de_marco</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TIPO_DE_MARCO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">radio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_attribute_sentido_de_apertura</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SENTIDO_DE_APERTURA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ext_attribute_id</t>
+    <t xml:space="preserve">attribute_id/id</t>
   </si>
   <si>
     <t xml:space="preserve">is_custom</t>
@@ -519,13 +505,10 @@
     <t xml:space="preserve">ALTO PL: 2400MM, ALTO MT: 2450MM</t>
   </si>
   <si>
-    <t xml:space="preserve">id</t>
-  </si>
-  <si>
     <t xml:space="preserve">description</t>
   </si>
   <si>
-    <t xml:space="preserve">ext_attribute_ids</t>
+    <t xml:space="preserve">attribute_line_ids/id</t>
   </si>
   <si>
     <t xml:space="preserve">product_template_rf_30_lite</t>
@@ -534,65 +517,16 @@
     <t xml:space="preserve">PUERTA RF30 LITE</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">product_attribute_ancho_pl_mt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">product_attribute_alto_pl_mt</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">product_template_rf_30_plus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PUERTA RF30 PLUS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_template_rf_60_lite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PUERTA RF60 LITE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_template_rf_60_plus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PUERTA RF60 PLUS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_template_rf_90_lite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PUERTA RF90 LITE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_template_rf_90_plus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PUERTA RF90 PLUS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_template_rf_120_lite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PUERTA RF120 LITE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_template_rf_120_plus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PUERTA RF120 PLUS</t>
+    <t xml:space="preserve">product_tmpl_id/id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value_ids/id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_template_rf_30_lite_attribute_line_ancho_pl_mt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_template_rf_30_lite_attribute_line_alto_pl_mt</t>
   </si>
 </sst>
 </file>
@@ -603,7 +537,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -624,11 +558,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -673,7 +602,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -690,15 +619,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -825,10 +746,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -859,7 +780,7 @@
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -873,39 +794,11 @@
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -927,7 +820,7 @@
   <dimension ref="A1:D75"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C37" activeCellId="0" sqref="C37"/>
+      <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -944,1119 +837,1119 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>15</v>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="5" t="n">
+      <c r="D2" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="5" t="n">
+      <c r="D3" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="5" t="n">
+      <c r="D4" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="5" t="n">
+      <c r="D5" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="5" t="n">
+      <c r="D6" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="5" t="n">
+      <c r="D7" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="5" t="n">
+      <c r="D8" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="5" t="n">
+      <c r="D9" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="5" t="n">
+      <c r="D10" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="5" t="n">
+      <c r="D11" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="5" t="n">
+      <c r="D12" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="5" t="n">
+      <c r="D13" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="5" t="n">
+      <c r="D14" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="5" t="n">
+      <c r="D15" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="5" t="n">
+      <c r="D16" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="5" t="n">
+      <c r="D17" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="5" t="n">
+      <c r="D18" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="5" t="n">
+      <c r="D19" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="5" t="n">
+      <c r="D20" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="5" t="n">
+      <c r="D21" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="5" t="n">
+      <c r="D22" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D23" s="5" t="n">
+      <c r="D23" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="5" t="n">
+      <c r="D24" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D25" s="5" t="n">
+      <c r="D25" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D26" s="5" t="n">
+      <c r="D26" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="5" t="n">
+      <c r="D27" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D28" s="5" t="n">
+      <c r="D28" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D29" s="5" t="n">
+      <c r="D29" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D30" s="5" t="n">
+      <c r="D30" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D31" s="5" t="n">
+      <c r="D31" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D32" s="5" t="n">
+      <c r="D32" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D33" s="5" t="n">
+      <c r="D33" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D34" s="5" t="n">
+      <c r="D34" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D35" s="5" t="n">
+      <c r="D35" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D36" s="5" t="n">
+      <c r="D36" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D37" s="5" t="n">
+      <c r="D37" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D38" s="5" t="n">
+      <c r="D38" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D39" s="5" t="n">
+      <c r="D39" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D40" s="5" t="n">
+      <c r="D40" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D41" s="5" t="n">
+      <c r="D41" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D42" s="5" t="n">
+      <c r="D42" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D43" s="5" t="n">
+      <c r="D43" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D44" s="5" t="n">
+      <c r="D44" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D45" s="5" t="n">
+      <c r="D45" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D46" s="5" t="n">
+      <c r="D46" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D47" s="5" t="n">
+      <c r="D47" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D48" s="5" t="n">
+      <c r="D48" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D49" s="5" t="n">
+      <c r="D49" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D50" s="5" t="n">
+      <c r="D50" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D51" s="5" t="n">
+      <c r="D51" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D52" s="5" t="n">
+      <c r="D52" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D53" s="5" t="n">
+      <c r="D53" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D54" s="5" t="n">
+      <c r="D54" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D55" s="5" t="n">
+      <c r="D55" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D56" s="5" t="n">
+      <c r="D56" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D57" s="5" t="n">
+      <c r="D57" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D58" s="5" t="n">
+      <c r="D58" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D59" s="5" t="n">
+      <c r="D59" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D60" s="5" t="n">
+      <c r="D60" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D61" s="5" t="n">
+      <c r="D61" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D62" s="5" t="n">
+      <c r="D62" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D63" s="5" t="n">
+      <c r="D63" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D64" s="5" t="n">
+      <c r="D64" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D65" s="5" t="n">
+      <c r="D65" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D66" s="5" t="n">
+      <c r="D66" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D67" s="5" t="n">
+      <c r="D67" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D68" s="5" t="n">
+      <c r="D68" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D69" s="5" t="n">
+      <c r="D69" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D70" s="5" t="n">
+      <c r="D70" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D71" s="5" t="n">
+      <c r="D71" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D72" s="5" t="n">
+      <c r="D72" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D73" s="5" t="n">
+      <c r="D73" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D74" s="5" t="n">
+      <c r="D74" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D75" s="5" t="n">
+      <c r="D75" s="4" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2077,10 +1970,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2088,133 +1981,36 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="33.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="109.62"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>165</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>167</v>
+        <v>160</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
+      </c>
+      <c r="D2" s="1" t="str">
+        <f aca="false">_xlfn.TEXTJOIN(",",1,'product.template.attribute.line'!A2:A3)</f>
+        <v>product_template_rf_30_lite_attribute_line_ancho_pl_mt,product_template_rf_30_lite_attribute_line_alto_pl_mt</v>
       </c>
     </row>
   </sheetData>
@@ -2226,4 +2022,79 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="52.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="29.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="29.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="59.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="47.3"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="str">
+        <f aca="false">_xlfn.TEXTJOIN(",",1,'product.attribute.value'!A2:A36)</f>
+        <v>product_attribute_value_ancho_pl_500_mt_600,product_attribute_value_ancho_pl_550_mt_650,product_attribute_value_ancho_pl_600_mt_700,product_attribute_value_ancho_pl_650_mt_750,product_attribute_value_ancho_pl_700_mt_800,product_attribute_value_ancho_pl_750_mt_850,product_attribute_value_ancho_pl_800_mt_900,product_attribute_value_ancho_pl_850_mt_950,product_attribute_value_ancho_pl_900_mt_1000,product_attribute_value_ancho_pl_950_mt_1050,product_attribute_value_ancho_pl_1000_mt_1100,product_attribute_value_ancho_pl_1050_mt_1150,product_attribute_value_ancho_pl_1100_mt_1200,product_attribute_value_ancho_pl_1150_mt_1250,product_attribute_value_ancho_pl_1200_mt_1300,product_attribute_value_ancho_pl_1250_mt_1350,product_attribute_value_ancho_pl_1300_mt_1400,product_attribute_value_ancho_pl_1350_mt_1450,product_attribute_value_ancho_pl_1400_mt_1500,product_attribute_value_ancho_pl_1450_mt_1550,product_attribute_value_ancho_pl_1500_mt_1600,product_attribute_value_ancho_pl_1550_mt_1650,product_attribute_value_ancho_pl_1600_mt_1700,product_attribute_value_ancho_pl_1650_mt_1750,product_attribute_value_ancho_pl_1700_mt_1800,product_attribute_value_ancho_pl_1750_mt_1850,product_attribute_value_ancho_pl_1800_mt_1900,product_attribute_value_ancho_pl_1850_mt_1950,product_attribute_value_ancho_pl_1900_mt_2000,product_attribute_value_ancho_pl_1950_mt_2050,product_attribute_value_ancho_pl_2000_mt_2100,product_attribute_value_ancho_pl_2050_mt_2150,product_attribute_value_ancho_pl_2100_mt_2200,product_attribute_value_ancho_pl_2150_mt_2250,product_attribute_value_ancho_pl_2200_mt_2300</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="str">
+        <f aca="false">_xlfn.TEXTJOIN(",",1,'product.attribute.value'!A37:A75)</f>
+        <v>product_attribute_value_alto_pl_500_mt_550,product_attribute_value_alto_pl_550_mt_600,product_attribute_value_alto_pl_600_mt_650,product_attribute_value_alto_pl_650_mt_700,product_attribute_value_alto_pl_700_mt_750,product_attribute_value_alto_pl_750_mt_800,product_attribute_value_alto_pl_800_mt_850,product_attribute_value_alto_pl_850_mt_900,product_attribute_value_alto_pl_900_mt_950,product_attribute_value_alto_pl_950_mt_1000,product_attribute_value_alto_pl_1000_mt_1050,product_attribute_value_alto_pl_1050_mt_1100,product_attribute_value_alto_pl_1100_mt_1150,product_attribute_value_alto_pl_1150_mt_1200,product_attribute_value_alto_pl_1200_mt_1250,product_attribute_value_alto_pl_1250_mt_1300,product_attribute_value_alto_pl_1300_mt_1350,product_attribute_value_alto_pl_1350_mt_1400,product_attribute_value_alto_pl_1400_mt_1450,product_attribute_value_alto_pl_1450_mt_1500,product_attribute_value_alto_pl_1500_mt_1550,product_attribute_value_alto_pl_1550_mt_1600,product_attribute_value_alto_pl_1600_mt_1650,product_attribute_value_alto_pl_1650_mt_1700,product_attribute_value_alto_pl_1700_mt_1750,product_attribute_value_alto_pl_1750_mt_1800,product_attribute_value_alto_pl_1800_mt_1850,product_attribute_value_alto_pl_1850_mt_1900,product_attribute_value_alto_pl_1900_mt_1950,product_attribute_value_alto_pl_1950_mt_2000,product_attribute_value_alto_pl_2000_mt_2050,product_attribute_value_alto_pl_2050_mt_2100,product_attribute_value_alto_pl_2100_mt_2150,product_attribute_value_alto_pl_2150_mt_2200,product_attribute_value_alto_pl_2200_mt_2250,product_attribute_value_alto_pl_2250_mt_2300,product_attribute_value_alto_pl_2300_mt_2350,product_attribute_value_alto_pl_2350_mt_2400,product_attribute_value_alto_pl_2400_mt_2450</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>